<commit_message>
added code for new services
</commit_message>
<xml_diff>
--- a/AWS_Progress_Tracker.xlsx
+++ b/AWS_Progress_Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\Desktop\AWS-terraform\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A71C66F-F172-4519-8BC0-5C180FCF86DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42588BEB-8A07-48FC-9D71-EDFAC59B58F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{2FA85890-BCA6-470A-8260-52EA0665D7EB}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="131">
   <si>
     <t xml:space="preserve">Start Date </t>
   </si>
@@ -437,6 +437,140 @@
   </si>
   <si>
     <t>https://github.com/ShivamGautam98/AWS-terraform/blob/main/AWS%20Services%20Actions.xlsx</t>
+  </si>
+  <si>
+    <t>Lambda
+S3
+SageMaker</t>
+  </si>
+  <si>
+    <t>Glacier</t>
+  </si>
+  <si>
+    <t>Archival storage
+Low cost storage for data not to be in use for long time
+Choice of storage class according to data retrieval requirements</t>
+  </si>
+  <si>
+    <t>QuickSight
+Sagemaker
+SNS</t>
+  </si>
+  <si>
+    <t>Created Glacier Vault from Console</t>
+  </si>
+  <si>
+    <t>Created Glacier Vault using terraform</t>
+  </si>
+  <si>
+    <t>https://github.com/ShivamGautam98/AWS-terraform/blob/main/glacier.tf</t>
+  </si>
+  <si>
+    <t>SageMaker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fully managed machine learning service
+One-click deployment
+More than 150 open source models
+</t>
+  </si>
+  <si>
+    <t>EC2
+RDS
+Lambda
+API Gateway
+VPC</t>
+  </si>
+  <si>
+    <t>EC2
+S3
+DNS
+Lambda
+SageMaker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Redshift
+Snowflare
+EMR
+LakeFormation
+QuickSight
+</t>
+  </si>
+  <si>
+    <t>EC2
+DynamoDb
+S3
+ECS
+EKS
+Lambda</t>
+  </si>
+  <si>
+    <t>Monitor and troubleshoot infrastructure
+Track and Visualize logs
+Anamalous behavior detection
+Set alarm based on some log triggers
+Take automated actions 
+Discover insights from logs, metrics and events
+Track resource health</t>
+  </si>
+  <si>
+    <t>Created a cloudWatch Dashboard resource using terraform</t>
+  </si>
+  <si>
+    <t>Created alarm for EC2 CPU utilization above threshold</t>
+  </si>
+  <si>
+    <t>CloudWatch
+Replication instance</t>
+  </si>
+  <si>
+    <t>CloudFormation Stack</t>
+  </si>
+  <si>
+    <t>S3 bucket
+CloudWatch</t>
+  </si>
+  <si>
+    <t>CloudWatch
+CloudTrail</t>
+  </si>
+  <si>
+    <t>CloudWatch
+S3 bucket</t>
+  </si>
+  <si>
+    <t>CloudTrail
+S3 bucket</t>
+  </si>
+  <si>
+    <t>https://github.com/ShivamGautam98/AWS-terraform/blob/main/cloudwatch.tf</t>
+  </si>
+  <si>
+    <t>API Gateway
+CloudFront
+ELB 
+LightSail
+Elastic Beanstalk
+EC2</t>
+  </si>
+  <si>
+    <t>CloudTrail
+Lambda
+Secrets Manager
+S3</t>
+  </si>
+  <si>
+    <t>DynamoDB
+Kinesis
+S3
+API Gateway
+SQS
+EventBridge
+EFS</t>
+  </si>
+  <si>
+    <t>EC2
+RDS</t>
   </si>
 </sst>
 </file>
@@ -511,10 +645,10 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -833,22 +967,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9BBF0D7-2510-401B-B670-F4C8700ABDF6}">
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.81640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="11.6328125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.453125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="24" style="1" customWidth="1"/>
-    <col min="5" max="5" width="14.90625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="12.26953125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="20.26953125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="12.90625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="16.54296875" style="1" customWidth="1"/>
-    <col min="10" max="10" width="15.54296875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="11.36328125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7265625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.6328125" style="1" customWidth="1"/>
+    <col min="4" max="10" width="19.81640625" style="1" customWidth="1"/>
     <col min="11" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
@@ -971,7 +1099,12 @@
       <c r="H4" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="I4" s="6"/>
+      <c r="I4" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="5" spans="1:10" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A5" s="3">
@@ -998,7 +1131,12 @@
       <c r="H5" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="I5" s="6"/>
+      <c r="I5" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="6" spans="1:10" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A6" s="3">
@@ -1025,7 +1163,12 @@
       <c r="H6" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="I6" s="6"/>
+      <c r="I6" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="7" spans="1:10" ht="145" x14ac:dyDescent="0.35">
       <c r="A7" s="3">
@@ -1050,11 +1193,13 @@
         <v>47</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="I7" s="6"/>
-    </row>
-    <row r="8" spans="1:10" ht="72.5" x14ac:dyDescent="0.35">
+        <v>121</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="87" x14ac:dyDescent="0.35">
       <c r="A8" s="3">
         <v>44627</v>
       </c>
@@ -1071,11 +1216,13 @@
         <v>44</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="I8" s="6"/>
-    </row>
-    <row r="9" spans="1:10" ht="58" x14ac:dyDescent="0.35">
+        <v>123</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="87" x14ac:dyDescent="0.35">
       <c r="A9" s="3">
         <v>44627</v>
       </c>
@@ -1098,9 +1245,14 @@
         <v>73</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="I9" s="6"/>
+        <v>122</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="10" spans="1:10" ht="174" x14ac:dyDescent="0.35">
       <c r="A10" s="3">
@@ -1125,9 +1277,11 @@
         <v>62</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="I10" s="6"/>
+        <v>123</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="11" spans="1:10" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A11" s="3">
@@ -1152,11 +1306,13 @@
         <v>42</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="I11" s="6"/>
+        <v>36</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>103</v>
+      </c>
       <c r="J11" s="1" t="s">
-        <v>36</v>
+        <v>128</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="87" x14ac:dyDescent="0.35">
@@ -1181,15 +1337,14 @@
       <c r="G12" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="H12" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="I12" s="6"/>
+      <c r="I12" s="5" t="s">
+        <v>103</v>
+      </c>
       <c r="J12" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="58" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" ht="87" x14ac:dyDescent="0.35">
       <c r="A13" s="3">
         <v>44624</v>
       </c>
@@ -1211,9 +1366,14 @@
       <c r="H13" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="I13" s="6"/>
-    </row>
-    <row r="14" spans="1:10" ht="87" x14ac:dyDescent="0.35">
+      <c r="I13" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A14" s="3">
         <v>44627</v>
       </c>
@@ -1238,9 +1398,14 @@
       <c r="H14" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="I14" s="6"/>
-    </row>
-    <row r="15" spans="1:10" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="I14" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="174" x14ac:dyDescent="0.35">
       <c r="A15" s="3">
         <v>44628</v>
       </c>
@@ -1263,16 +1428,21 @@
         <v>83</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="I15" s="6"/>
+        <v>120</v>
+      </c>
+      <c r="I15" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="16" spans="1:10" ht="145" x14ac:dyDescent="0.35">
       <c r="A16" s="3">
         <v>44629</v>
       </c>
       <c r="B16" s="3">
-        <v>44630</v>
+        <v>44629</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>76</v>
@@ -1292,17 +1462,19 @@
       <c r="H16" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="I16" s="6"/>
+      <c r="I16" s="5" t="s">
+        <v>103</v>
+      </c>
       <c r="J16" s="1" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A17" s="3">
-        <v>44630</v>
+        <v>44629</v>
       </c>
       <c r="B17" s="3">
-        <v>44630</v>
+        <v>44629</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>85</v>
@@ -1319,7 +1491,12 @@
       <c r="G17" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="I17" s="6"/>
+      <c r="H17" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="I17" s="5" t="s">
+        <v>103</v>
+      </c>
       <c r="J17" s="1" t="s">
         <v>86</v>
       </c>
@@ -1346,12 +1523,17 @@
       <c r="G18" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="I18" s="6"/>
+      <c r="H18" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="I18" s="5" t="s">
+        <v>103</v>
+      </c>
       <c r="J18" s="1" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" ht="87" x14ac:dyDescent="0.35">
       <c r="A19" s="3">
         <v>44630</v>
       </c>
@@ -1373,19 +1555,105 @@
       <c r="G19" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="I19" s="6"/>
+      <c r="H19" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="I19" s="5" t="s">
+        <v>103</v>
+      </c>
       <c r="J19" s="1" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="I20" s="6"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="I21" s="6"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="I22" s="6"/>
+    <row r="20" spans="1:10" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A20" s="3">
+        <v>44630</v>
+      </c>
+      <c r="B20" s="3">
+        <v>44630</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="I20" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="87" x14ac:dyDescent="0.35">
+      <c r="A21" s="3">
+        <v>44630</v>
+      </c>
+      <c r="B21" s="3">
+        <v>44630</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="I21" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="159.5" x14ac:dyDescent="0.35">
+      <c r="A22" s="3">
+        <v>44630</v>
+      </c>
+      <c r="B22" s="3">
+        <v>44630</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="I22" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.35">
       <c r="I23" s="6"/>
@@ -1403,9 +1671,6 @@
       <c r="I27" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="I3:I27"/>
-  </mergeCells>
   <hyperlinks>
     <hyperlink ref="G5" r:id="rId1" xr:uid="{2A3A4F26-C4D0-479D-9817-AB4C393A665D}"/>
     <hyperlink ref="G2" r:id="rId2" xr:uid="{31D7CC19-C5B0-423E-B891-6C9E2E6CC363}"/>
@@ -1424,8 +1689,12 @@
     <hyperlink ref="G18" r:id="rId15" xr:uid="{F13C23EF-805F-402D-BC99-F4B4688415EF}"/>
     <hyperlink ref="G19" r:id="rId16" xr:uid="{3F0EC9AE-FBA8-455A-8B49-DAE1EFE44771}"/>
     <hyperlink ref="I3" r:id="rId17" xr:uid="{0EA5DE86-A4F6-40BE-B296-AAD55A78B618}"/>
+    <hyperlink ref="G20" r:id="rId18" xr:uid="{73E5A990-B37A-45F6-A316-D0E97EC3DD88}"/>
+    <hyperlink ref="G22" r:id="rId19" xr:uid="{0B7B7FA2-BD72-446E-B3F8-70584586B5FC}"/>
+    <hyperlink ref="I4" r:id="rId20" xr:uid="{09EB1D13-C603-4FF9-A63B-D690BB35C7AC}"/>
+    <hyperlink ref="I5:I22" r:id="rId21" display="https://github.com/ShivamGautam98/AWS-terraform/blob/main/AWS%20Services%20Actions.xlsx" xr:uid="{4E8B50E3-05D1-4F72-AB8B-9F807CE11285}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId18"/>
+  <pageSetup orientation="portrait" r:id="rId22"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added elasticahe and beanstalk
</commit_message>
<xml_diff>
--- a/AWS_Progress_Tracker.xlsx
+++ b/AWS_Progress_Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\Desktop\AWS-terraform\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B23560D-A642-4601-A89B-CF111C92A734}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFB4F5BB-48C1-4F10-8229-9A10FA9126DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{2FA85890-BCA6-470A-8260-52EA0665D7EB}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="174">
   <si>
     <t xml:space="preserve">Start Date </t>
   </si>
@@ -66,16 +66,6 @@
   </si>
   <si>
     <t>EC2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Virtual machine.
-Ssh
-Freedom for any OS
-Compute resource on the fly
-Choice of Processors
-Choice of resource location
-Placement groups
-</t>
   </si>
   <si>
     <t xml:space="preserve">Created t2.micro EC2 instance in Asia Pacific (Mumbai) region </t>
@@ -686,6 +676,85 @@
   </si>
   <si>
     <t>https://github.com/ShivamGautam98/AWS-terraform/blob/main/codetrail.tf</t>
+  </si>
+  <si>
+    <t>Workspaces</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cloud Hosting
+Ssh
+Freedom for any OS
+Compute resource on the fly
+Choice of Processors
+Choice of resource location
+Placement groups
+</t>
+  </si>
+  <si>
+    <t>Virtual Desktop
+Easily provision cloud-based desktops that allow end-users to access applications and resources
+Facilitate remote work</t>
+  </si>
+  <si>
+    <t>S3
+Cloud9</t>
+  </si>
+  <si>
+    <t>Elasticache</t>
+  </si>
+  <si>
+    <t>In-memory caching service
+Compatible with Redis and Memcached
+Used where frequently accessed data must be in-memory.
+Caching
+Session store</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EMR
+SageMaker
+EC2
+Kinesis
+Kafka
+Lambda
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Created a Memcache node of type cache.t2.micro </t>
+  </si>
+  <si>
+    <t>Created a RedisCache node of type cache.t2.micro using terraform</t>
+  </si>
+  <si>
+    <t>Beanstalk</t>
+  </si>
+  <si>
+    <t>https://github.com/ShivamGautam98/AWS-terraform/blob/main/elasticache.tf</t>
+  </si>
+  <si>
+    <t>Automatic Deployment
+End-to-end web application management
+Service for deploying and scaling web applications and services</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Created sample python application using Elastic Beanstalk </t>
+  </si>
+  <si>
+    <t>Created Beanstalk application using terraform</t>
+  </si>
+  <si>
+    <t>https://github.com/ShivamGautam98/AWS-terraform/blob/main/elasticbeanstalk.tf</t>
+  </si>
+  <si>
+    <t>EC2
+Lambda
+S3
+CloudFront
+EventBridge
+DynamoDB
+ElastiCache
+EFS
+RDS
+VPC</t>
   </si>
 </sst>
 </file>
@@ -1070,10 +1139,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9BBF0D7-2510-401B-B670-F4C8700ABDF6}">
-  <dimension ref="A1:J28"/>
+  <dimension ref="A1:J31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1128,25 +1197,25 @@
         <v>10</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="F2" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="130.5" x14ac:dyDescent="0.35">
@@ -1157,28 +1226,28 @@
         <v>44623</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F3" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="G3" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>60</v>
-      </c>
       <c r="I3" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="87" x14ac:dyDescent="0.35">
@@ -1189,29 +1258,29 @@
         <v>44623</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="E4" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>58</v>
       </c>
       <c r="G4" s="4"/>
       <c r="H4" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I4" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="J4" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="J4" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="101.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="5" spans="1:10" ht="87" x14ac:dyDescent="0.35">
       <c r="A5" s="3">
         <v>44624</v>
       </c>
@@ -1219,31 +1288,31 @@
         <v>44624</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="F5" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="130.5" x14ac:dyDescent="0.35">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A6" s="3">
         <v>44624</v>
       </c>
@@ -1251,31 +1320,31 @@
         <v>44624</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>20</v>
-      </c>
       <c r="F6" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="145" x14ac:dyDescent="0.35">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="188.5" x14ac:dyDescent="0.35">
       <c r="A7" s="3">
         <v>44624</v>
       </c>
@@ -1283,28 +1352,28 @@
         <v>44624</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>23</v>
-      </c>
       <c r="F7" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G7" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="G7" s="4" t="s">
-        <v>47</v>
-      </c>
       <c r="H7" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="87" x14ac:dyDescent="0.35">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A8" s="3">
         <v>44627</v>
       </c>
@@ -1312,19 +1381,19 @@
         <v>44627</v>
       </c>
       <c r="C8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="E8" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="87" x14ac:dyDescent="0.35">
@@ -1335,31 +1404,31 @@
         <v>44627</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F9" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="G9" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="G9" s="4" t="s">
-        <v>73</v>
-      </c>
       <c r="H9" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="174" x14ac:dyDescent="0.35">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="203" x14ac:dyDescent="0.35">
       <c r="A10" s="3">
         <v>44627</v>
       </c>
@@ -1367,28 +1436,28 @@
         <v>44627</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="E10" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E10" s="1" t="s">
-        <v>32</v>
-      </c>
       <c r="F10" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G10" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="G10" s="4" t="s">
-        <v>62</v>
-      </c>
       <c r="H10" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="101.5" x14ac:dyDescent="0.35">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="116" x14ac:dyDescent="0.35">
       <c r="A11" s="3">
         <v>44628</v>
       </c>
@@ -1396,31 +1465,31 @@
         <v>44628</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="E11" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="H11" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E11" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="I11" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="87" x14ac:dyDescent="0.35">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="116" x14ac:dyDescent="0.35">
       <c r="A12" s="3">
         <v>44622</v>
       </c>
@@ -1428,28 +1497,28 @@
         <v>44622</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D12" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="J12" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E12" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="I12" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="J12" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="87" x14ac:dyDescent="0.35">
+    </row>
+    <row r="13" spans="1:10" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A13" s="3">
         <v>44624</v>
       </c>
@@ -1457,22 +1526,22 @@
         <v>44624</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F13" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="G13" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="G13" s="4" t="s">
-        <v>70</v>
-      </c>
       <c r="H13" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I13" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J13" s="1" t="s">
         <v>10</v>
@@ -1486,28 +1555,28 @@
         <v>44627</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I14" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="174" x14ac:dyDescent="0.35">
@@ -1518,31 +1587,31 @@
         <v>44628</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I15" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="145" x14ac:dyDescent="0.35">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="188.5" x14ac:dyDescent="0.35">
       <c r="A16" s="3">
         <v>44629</v>
       </c>
@@ -1550,28 +1619,28 @@
         <v>44629</v>
       </c>
       <c r="C16" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="I16" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="J16" s="1" t="s">
         <v>76</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="G16" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="I16" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="J16" s="1" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="101.5" x14ac:dyDescent="0.35">
@@ -1582,31 +1651,31 @@
         <v>44629</v>
       </c>
       <c r="C17" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="I17" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="J17" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="D17" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="G17" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="I17" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="J17" s="1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="130.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="18" spans="1:10" ht="145" x14ac:dyDescent="0.35">
       <c r="A18" s="3">
         <v>44630</v>
       </c>
@@ -1614,31 +1683,31 @@
         <v>44630</v>
       </c>
       <c r="C18" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="I18" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="J18" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="D18" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="G18" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="I18" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="J18" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="87" x14ac:dyDescent="0.35">
+    </row>
+    <row r="19" spans="1:10" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A19" s="3">
         <v>44630</v>
       </c>
@@ -1646,28 +1715,28 @@
         <v>44630</v>
       </c>
       <c r="C19" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="E19" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="I19" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="J19" s="1" t="s">
         <v>98</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="G19" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="I19" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="J19" s="1" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="101.5" x14ac:dyDescent="0.35">
@@ -1678,31 +1747,31 @@
         <v>44630</v>
       </c>
       <c r="C20" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="E20" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I20" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="J20" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="E20" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="G20" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="H20" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="I20" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="J20" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" ht="87" x14ac:dyDescent="0.35">
+    </row>
+    <row r="21" spans="1:10" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A21" s="3">
         <v>44630</v>
       </c>
@@ -1710,25 +1779,25 @@
         <v>44630</v>
       </c>
       <c r="C21" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D21" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="D21" s="1" t="s">
-        <v>112</v>
-      </c>
       <c r="E21" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I21" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" ht="159.5" x14ac:dyDescent="0.35">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="217.5" x14ac:dyDescent="0.35">
       <c r="A22" s="3">
         <v>44630</v>
       </c>
@@ -1736,28 +1805,28 @@
         <v>44630</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D22" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="F22" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="E22" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>118</v>
-      </c>
       <c r="G22" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I22" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="116" x14ac:dyDescent="0.35">
@@ -1768,22 +1837,22 @@
         <v>44631</v>
       </c>
       <c r="C23" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D23" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="F23" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="I23" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="J23" s="1" t="s">
         <v>132</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="G23" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="I23" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="J23" s="1" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="72.5" x14ac:dyDescent="0.35">
@@ -1794,25 +1863,25 @@
         <v>44631</v>
       </c>
       <c r="C24" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D24" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="D24" s="1" t="s">
-        <v>136</v>
-      </c>
       <c r="F24" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="G24" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="G24" s="4" t="s">
+      <c r="H24" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="H24" s="1" t="s">
-        <v>140</v>
-      </c>
       <c r="I24" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="72.5" x14ac:dyDescent="0.35">
@@ -1823,25 +1892,28 @@
         <v>44631</v>
       </c>
       <c r="C25" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I25" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="J25" s="1" t="s">
         <v>141</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="H25" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="I25" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="J25" s="1" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="72.5" x14ac:dyDescent="0.35">
@@ -1852,25 +1924,28 @@
         <v>44631</v>
       </c>
       <c r="C26" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="D26" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="E26" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I26" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="J26" s="1" t="s">
         <v>146</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="H26" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="I26" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="J26" s="1" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="232" x14ac:dyDescent="0.35">
@@ -1881,28 +1956,28 @@
         <v>44634</v>
       </c>
       <c r="C27" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="D27" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="D27" s="1" t="s">
+      <c r="E27" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="I27" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="J27" s="1" t="s">
         <v>149</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="G27" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="H27" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="I27" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="J27" s="1" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="72.5" x14ac:dyDescent="0.35">
@@ -1913,28 +1988,121 @@
         <v>44634</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D28" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="G28" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="I28" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="J28" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="E28" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="G28" s="4" t="s">
+    </row>
+    <row r="29" spans="1:10" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A29" s="3">
+        <v>44635</v>
+      </c>
+      <c r="B29" s="3">
+        <v>44635</v>
+      </c>
+      <c r="C29" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="H28" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="I28" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="J28" s="1" t="s">
-        <v>155</v>
+      <c r="D29" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" ht="145" x14ac:dyDescent="0.35">
+      <c r="A30" s="3">
+        <v>44636</v>
+      </c>
+      <c r="B30" s="3">
+        <v>44636</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="G30" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="I30" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="J30" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" ht="145" x14ac:dyDescent="0.35">
+      <c r="A31" s="3">
+        <v>44636</v>
+      </c>
+      <c r="B31" s="3">
+        <v>44636</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="G31" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="I31" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="J31" s="1" t="s">
+        <v>173</v>
       </c>
     </row>
   </sheetData>
@@ -1970,8 +2138,12 @@
     <hyperlink ref="I27" r:id="rId29" xr:uid="{7B843C1F-ED9B-43BB-BB6B-B1BB98384675}"/>
     <hyperlink ref="G28" r:id="rId30" xr:uid="{04C5685F-80EF-41C5-9558-46D63C3389F5}"/>
     <hyperlink ref="I28" r:id="rId31" xr:uid="{422C1E3C-AFBA-40CF-A60F-6362EDF69A34}"/>
+    <hyperlink ref="I30" r:id="rId32" xr:uid="{16C4F23A-E405-4474-8CE0-0FBA1BA2C30C}"/>
+    <hyperlink ref="G30" r:id="rId33" xr:uid="{0ECA6433-B4AB-4C95-A46C-D1509FD58F3C}"/>
+    <hyperlink ref="G31" r:id="rId34" xr:uid="{72F58137-7720-48E5-AF61-417DE8B2AC7B}"/>
+    <hyperlink ref="I31" r:id="rId35" xr:uid="{8618B8C6-88AD-48FD-9226-6EA6C4D7EAAF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId32"/>
+  <pageSetup orientation="portrait" r:id="rId36"/>
 </worksheet>
 </file>
</xml_diff>